<commit_message>
added 2d plots for dimension sweep
</commit_message>
<xml_diff>
--- a/FEMM Simulations/Data/DimensionSweep 2019_10_31 22_09 (Length Sweep)/R0.1 swLength.xlsx
+++ b/FEMM Simulations/Data/DimensionSweep 2019_10_31 22_09 (Length Sweep)/R0.1 swLength.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekultho\Documents\Personal\CG 490\FEMM Simulations\Data\DimensionSweep 2019_10_31 22_09 (Length Sweep)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas Kulin\Documents\Projects\CG-490\FEMM Simulations\Data\DimensionSweep 2019_10_31 22_09 (Length Sweep)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844602BF-591A-49A5-8658-70201B287C56}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7947EF40-C034-4B33-8BDB-99644C8D0BB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Force vs. Position" sheetId="1" r:id="rId1"/>
+    <sheet name="Coil vs. Inductance" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -28,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
   <si>
     <t>Position [cm]</t>
   </si>
@@ -156,10 +160,52 @@
     <t>MAX E</t>
   </si>
   <si>
-    <t>Velocity [m/s]</t>
+    <t>Coil Geometry</t>
   </si>
   <si>
-    <t>Energy [J]</t>
+    <t>Inductance [uH]</t>
+  </si>
+  <si>
+    <t>len = 10.0 mm rad = 4.0 mm</t>
+  </si>
+  <si>
+    <t>len = 20.0 mm rad = 4.0 mm</t>
+  </si>
+  <si>
+    <t>len = 30.0 mm rad = 4.0 mm</t>
+  </si>
+  <si>
+    <t>len = 40.0 mm rad = 4.0 mm</t>
+  </si>
+  <si>
+    <t>len = 50.0 mm rad = 4.0 mm</t>
+  </si>
+  <si>
+    <t>len = 60.0 mm rad = 4.0 mm</t>
+  </si>
+  <si>
+    <t>len = 70.0 mm rad = 4.0 mm</t>
+  </si>
+  <si>
+    <t>len = 80.0 mm rad = 4.0 mm</t>
+  </si>
+  <si>
+    <t>len = 90.0 mm rad = 4.0 mm</t>
+  </si>
+  <si>
+    <t>len = 100.0 mm rad = 4.0 mm</t>
+  </si>
+  <si>
+    <t>R0.1 Velocity [m/s]</t>
+  </si>
+  <si>
+    <t>R0.1 Energy [J]</t>
+  </si>
+  <si>
+    <t>L40 Velocity [m/s]</t>
+  </si>
+  <si>
+    <t>L40 Energy [J]</t>
   </si>
 </sst>
 </file>
@@ -327,7 +373,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>'Force vs. Position'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -362,7 +408,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>'Force vs. Position'!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -404,7 +450,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:f>'Force vs. Position'!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -456,7 +502,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>'Force vs. Position'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -491,7 +537,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>'Force vs. Position'!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -533,7 +579,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$12</c:f>
+              <c:f>'Force vs. Position'!$C$2:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -585,7 +631,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>'Force vs. Position'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -620,7 +666,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>'Force vs. Position'!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -662,7 +708,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$12</c:f>
+              <c:f>'Force vs. Position'!$D$2:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -714,7 +760,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>'Force vs. Position'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -749,7 +795,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>'Force vs. Position'!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -791,7 +837,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$12</c:f>
+              <c:f>'Force vs. Position'!$E$2:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -843,7 +889,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>'Force vs. Position'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -878,7 +924,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>'Force vs. Position'!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -920,7 +966,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$12</c:f>
+              <c:f>'Force vs. Position'!$F$2:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -972,7 +1018,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>'Force vs. Position'!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1007,7 +1053,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>'Force vs. Position'!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1049,7 +1095,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$12</c:f>
+              <c:f>'Force vs. Position'!$G$2:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1101,7 +1147,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
+              <c:f>'Force vs. Position'!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1142,7 +1188,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>'Force vs. Position'!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1184,7 +1230,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$12</c:f>
+              <c:f>'Force vs. Position'!$H$2:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1236,7 +1282,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$1</c:f>
+              <c:f>'Force vs. Position'!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1277,7 +1323,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>'Force vs. Position'!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1319,7 +1365,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$12</c:f>
+              <c:f>'Force vs. Position'!$I$2:$I$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1371,7 +1417,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$1</c:f>
+              <c:f>'Force vs. Position'!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1412,7 +1458,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>'Force vs. Position'!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1454,7 +1500,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$12</c:f>
+              <c:f>'Force vs. Position'!$J$2:$J$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1506,7 +1552,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$1</c:f>
+              <c:f>'Force vs. Position'!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1547,7 +1593,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>'Force vs. Position'!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1589,7 +1635,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$K$2:$K$12</c:f>
+              <c:f>'Force vs. Position'!$K$2:$K$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2086,7 +2132,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$33</c:f>
+              <c:f>'Force vs. Position'!$B$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2121,7 +2167,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$34:$A$46</c:f>
+              <c:f>'Force vs. Position'!$A$34:$A$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2169,7 +2215,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$34:$B$46</c:f>
+              <c:f>'Force vs. Position'!$B$34:$B$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2227,7 +2273,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$33</c:f>
+              <c:f>'Force vs. Position'!$C$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2262,7 +2308,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$34:$A$46</c:f>
+              <c:f>'Force vs. Position'!$A$34:$A$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2310,7 +2356,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$34:$C$46</c:f>
+              <c:f>'Force vs. Position'!$C$34:$C$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2368,7 +2414,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$33</c:f>
+              <c:f>'Force vs. Position'!$D$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2403,7 +2449,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$34:$A$46</c:f>
+              <c:f>'Force vs. Position'!$A$34:$A$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2451,7 +2497,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$34:$D$46</c:f>
+              <c:f>'Force vs. Position'!$D$34:$D$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2509,7 +2555,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$33</c:f>
+              <c:f>'Force vs. Position'!$E$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2544,7 +2590,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$34:$A$46</c:f>
+              <c:f>'Force vs. Position'!$A$34:$A$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2592,7 +2638,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$34:$E$46</c:f>
+              <c:f>'Force vs. Position'!$E$34:$E$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2650,7 +2696,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$33</c:f>
+              <c:f>'Force vs. Position'!$F$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2685,7 +2731,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$34:$A$46</c:f>
+              <c:f>'Force vs. Position'!$A$34:$A$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2733,7 +2779,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$34:$F$46</c:f>
+              <c:f>'Force vs. Position'!$F$34:$F$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2791,7 +2837,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$33</c:f>
+              <c:f>'Force vs. Position'!$G$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2826,7 +2872,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$34:$A$46</c:f>
+              <c:f>'Force vs. Position'!$A$34:$A$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2874,7 +2920,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$34:$G$46</c:f>
+              <c:f>'Force vs. Position'!$G$34:$G$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2932,7 +2978,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$33</c:f>
+              <c:f>'Force vs. Position'!$H$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2973,7 +3019,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$34:$A$46</c:f>
+              <c:f>'Force vs. Position'!$A$34:$A$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3021,7 +3067,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$34:$H$46</c:f>
+              <c:f>'Force vs. Position'!$H$34:$H$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3079,7 +3125,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$33</c:f>
+              <c:f>'Force vs. Position'!$I$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3120,7 +3166,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$34:$A$46</c:f>
+              <c:f>'Force vs. Position'!$A$34:$A$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3168,7 +3214,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$34:$I$46</c:f>
+              <c:f>'Force vs. Position'!$I$34:$I$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3226,7 +3272,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$33</c:f>
+              <c:f>'Force vs. Position'!$J$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3267,7 +3313,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$34:$A$46</c:f>
+              <c:f>'Force vs. Position'!$A$34:$A$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3315,7 +3361,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$34:$J$46</c:f>
+              <c:f>'Force vs. Position'!$J$34:$J$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3373,7 +3419,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$33</c:f>
+              <c:f>'Force vs. Position'!$K$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3414,7 +3460,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$34:$A$46</c:f>
+              <c:f>'Force vs. Position'!$A$34:$A$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3462,7 +3508,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$K$34:$K$46</c:f>
+              <c:f>'Force vs. Position'!$K$34:$K$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3897,7 +3943,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17206531853227544"/>
+          <c:x val="0.25458103266826859"/>
           <c:y val="3.6629763322896108E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3917,8 +3963,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.3670878349508634E-2"/>
-          <c:y val="0.14374236874236876"/>
+          <c:x val="8.3670809989932357E-2"/>
+          <c:y val="0.1401117820550094"/>
           <c:w val="0.82192015791605066"/>
           <c:h val="0.65593513980363038"/>
         </c:manualLayout>
@@ -3931,11 +3977,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$58</c:f>
+              <c:f>'Force vs. Position'!$B$58</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Velocity [m/s]</c:v>
+                  <c:v>R0.1 Velocity [m/s]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3966,7 +4012,7 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Sheet1!$A$59:$A$68</c:f>
+              <c:f>'Force vs. Position'!$A$59:$A$68</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -4004,7 +4050,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$59:$B$68</c:f>
+              <c:f>'Force vs. Position'!$B$59:$B$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4045,6 +4091,104 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000F-6407-4D96-B234-51B654C8AF18}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Force vs. Position'!$D$58</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>L40 Velocity [m/s]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:strRef>
+              <c:f>'Force vs. Position'!$A$59:$A$68</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1 cm </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 cm </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3 cm</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4 cm </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5 cm </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6 cm </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7 cm</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8 cm </c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9 cm </c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10 cm </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Force vs. Position'!$D$59:$D$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>13.630141578818929</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.41793226250881</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.406716488533981</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.829682422442303</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.459804646745468</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.725289492116069</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.084701907070789</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.553135665548929</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.059121015447513</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.510721826072064</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-4E2F-4E7B-8F06-DB07BA041244}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4067,11 +4211,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$58</c:f>
+              <c:f>'Force vs. Position'!$C$58</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Energy [J]</c:v>
+                  <c:v>R0.1 Energy [J]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4102,7 +4246,7 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Sheet1!$A$59:$A$68</c:f>
+              <c:f>'Force vs. Position'!$A$59:$A$68</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -4140,7 +4284,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$59:$C$68</c:f>
+              <c:f>'Force vs. Position'!$C$59:$C$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4181,6 +4325,104 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000011-6407-4D96-B234-51B654C8AF18}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Force vs. Position'!$E$58</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>L40 Energy [J]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:strRef>
+              <c:f>'Force vs. Position'!$A$59:$A$68</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1 cm </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 cm </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3 cm</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4 cm </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5 cm </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6 cm </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7 cm</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8 cm </c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9 cm </c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10 cm </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Force vs. Position'!$E$59:$E$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.47511821411102051</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2158589841201031</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.82113601164577</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2497001572577777</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6735961153807559</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.8906480860794654</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0649729931017586</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2240025580392877</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.3471468154077755</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.3884888682617169</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-4E2F-4E7B-8F06-DB07BA041244}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4512,10 +4754,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.30626869315754141"/>
-          <c:y val="0.92518315018315012"/>
-          <c:w val="0.39721967893548188"/>
-          <c:h val="6.0287656350648477E-2"/>
+          <c:x val="0.18148877876580766"/>
+          <c:y val="0.91066068963427416"/>
+          <c:w val="0.59646502479354035"/>
+          <c:h val="7.4816962673850088E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -5758,16 +6000,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>107155</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>866775</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>45242</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>357188</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5793,6 +6035,140 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Force vs. Position"/>
+      <sheetName val="Coil vs. Inductance"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="58">
+          <cell r="B58" t="str">
+            <v>L40 Velocity [m/s]</v>
+          </cell>
+          <cell r="C58" t="str">
+            <v>L40 Energy [J]</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="A59" t="str">
+            <v xml:space="preserve">1 cm </v>
+          </cell>
+          <cell r="B59">
+            <v>13.630141578818929</v>
+          </cell>
+          <cell r="C59">
+            <v>0.47511821411102051</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="A60" t="str">
+            <v xml:space="preserve">2 cm </v>
+          </cell>
+          <cell r="B60">
+            <v>15.41793226250881</v>
+          </cell>
+          <cell r="C60">
+            <v>1.2158589841201031</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="A61" t="str">
+            <v>3 cm</v>
+          </cell>
+          <cell r="B61">
+            <v>15.406716488533981</v>
+          </cell>
+          <cell r="C61">
+            <v>1.82113601164577</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="A62" t="str">
+            <v xml:space="preserve">4 cm </v>
+          </cell>
+          <cell r="B62">
+            <v>14.829682422442303</v>
+          </cell>
+          <cell r="C62">
+            <v>2.2497001572577777</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="A63" t="str">
+            <v xml:space="preserve">5 cm </v>
+          </cell>
+          <cell r="B63">
+            <v>14.459804646745468</v>
+          </cell>
+          <cell r="C63">
+            <v>2.6735961153807559</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="A64" t="str">
+            <v xml:space="preserve">6 cm </v>
+          </cell>
+          <cell r="B64">
+            <v>13.725289492116069</v>
+          </cell>
+          <cell r="C64">
+            <v>2.8906480860794654</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="A65" t="str">
+            <v>7 cm</v>
+          </cell>
+          <cell r="B65">
+            <v>13.084701907070789</v>
+          </cell>
+          <cell r="C65">
+            <v>3.0649729931017586</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="A66" t="str">
+            <v xml:space="preserve">8 cm </v>
+          </cell>
+          <cell r="B66">
+            <v>12.553135665548929</v>
+          </cell>
+          <cell r="C66">
+            <v>3.2240025580392877</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="A67" t="str">
+            <v xml:space="preserve">9 cm </v>
+          </cell>
+          <cell r="B67">
+            <v>12.059121015447513</v>
+          </cell>
+          <cell r="C67">
+            <v>3.3471468154077755</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="A68" t="str">
+            <v xml:space="preserve">10 cm </v>
+          </cell>
+          <cell r="B68">
+            <v>11.510721826072064</v>
+          </cell>
+          <cell r="C68">
+            <v>3.3884888682617169</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6118,53 +6494,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="7.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1328125" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="11.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>-2</v>
       </c>
@@ -6199,7 +6575,7 @@
         <v>1.8339784352603791E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>-1</v>
       </c>
@@ -6234,7 +6610,7 @@
         <v>0.1153148505727849</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>0</v>
       </c>
@@ -6269,7 +6645,7 @@
         <v>4.1588473329984632</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1</v>
       </c>
@@ -6304,7 +6680,7 @@
         <v>33.937935282452322</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>2</v>
       </c>
@@ -6339,7 +6715,7 @@
         <v>36.869492010558602</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>3</v>
       </c>
@@ -6374,7 +6750,7 @@
         <v>37.43400287405175</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>4</v>
       </c>
@@ -6409,7 +6785,7 @@
         <v>37.37246407057178</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>5</v>
       </c>
@@ -6444,7 +6820,7 @@
         <v>37.236614751510267</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>6</v>
       </c>
@@ -6479,7 +6855,7 @@
         <v>36.634543853839901</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>7</v>
       </c>
@@ -6514,7 +6890,7 @@
         <v>36.415627291054953</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>8</v>
       </c>
@@ -6549,7 +6925,7 @@
         <v>35.089770238955573</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
@@ -6566,7 +6942,7 @@
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -6610,7 +6986,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>-2</v>
       </c>
@@ -6655,7 +7031,7 @@
         <v>1.8339784352603791E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>-1</v>
       </c>
@@ -6700,7 +7076,7 @@
         <v>1.8339784352603791E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>0</v>
       </c>
@@ -6745,7 +7121,7 @@
         <v>1.336546349253887E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>1</v>
       </c>
@@ -6790,7 +7166,7 @@
         <v>4.2925019679238521E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>2</v>
       </c>
@@ -6835,7 +7211,7 @@
         <v>0.38230437250376176</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>3</v>
       </c>
@@ -6880,7 +7256,7 @@
         <v>0.75099929260934772</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>4</v>
       </c>
@@ -6925,7 +7301,7 @@
         <v>1.1253393213498653</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>5</v>
       </c>
@@ -6970,7 +7346,7 @@
         <v>1.4990639620555828</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>6</v>
       </c>
@@ -7015,7 +7391,7 @@
         <v>1.8714301095706856</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>7</v>
       </c>
@@ -7060,7 +7436,7 @@
         <v>2.2377755481090844</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>8</v>
       </c>
@@ -7105,7 +7481,7 @@
         <v>2.6019318210196336</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>9</v>
       </c>
@@ -7150,7 +7526,7 @@
         <v>2.9528295234091892</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>10</v>
       </c>
@@ -7195,7 +7571,7 @@
         <v>2.9528295234091892</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B32" s="3" t="s">
         <v>35</v>
       </c>
@@ -7209,7 +7585,7 @@
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
@@ -7244,7 +7620,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>-2</v>
       </c>
@@ -7289,7 +7665,7 @@
         <v>8.4683078847678672E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>-1</v>
       </c>
@@ -7334,7 +7710,7 @@
         <v>8.4683078847678672E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>0</v>
       </c>
@@ -7379,7 +7755,7 @@
         <v>0.22860806044484211</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>1</v>
       </c>
@@ -7424,7 +7800,7 @@
         <v>1.2955517894372903</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>2</v>
       </c>
@@ -7469,7 +7845,7 @@
         <v>3.8663766526623733</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>3</v>
       </c>
@@ -7514,7 +7890,7 @@
         <v>5.4190017467700571</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>4</v>
       </c>
@@ -7559,7 +7935,7 @@
         <v>6.6334777095138664</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>5</v>
       </c>
@@ -7604,7 +7980,7 @@
         <v>7.65613546159019</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>6</v>
       </c>
@@ -7649,7 +8025,7 @@
         <v>8.5543365656820924</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>7</v>
       </c>
@@ -7694,7 +8070,7 @@
         <v>9.354224507914898</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>8</v>
       </c>
@@ -7739,7 +8115,7 @@
         <v>10.086662353787062</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>9</v>
       </c>
@@ -7784,7 +8160,7 @@
         <v>10.745304184196016</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>10</v>
       </c>
@@ -7829,7 +8205,7 @@
         <v>10.745304184196016</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>40</v>
       </c>
@@ -7874,7 +8250,7 @@
         <v>10.745304184196016</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>41</v>
       </c>
@@ -7919,7 +8295,7 @@
         <v>2.9528295234091897</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C51" s="1" t="s">
         <v>36</v>
       </c>
@@ -7927,7 +8303,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C52">
         <v>8040</v>
       </c>
@@ -7935,7 +8311,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>38</v>
       </c>
@@ -7970,7 +8346,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>39</v>
       </c>
@@ -8015,18 +8391,24 @@
         <v>5.1148269120599998E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>43</v>
+        <v>55</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A59" s="2" t="s">
         <v>25</v>
       </c>
@@ -8036,8 +8418,14 @@
       <c r="C59">
         <v>0.68027915099734881</v>
       </c>
+      <c r="D59">
+        <v>13.630141578818929</v>
+      </c>
+      <c r="E59">
+        <v>0.47511821411102051</v>
+      </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A60" s="2" t="s">
         <v>26</v>
       </c>
@@ -8047,8 +8435,14 @@
       <c r="C60">
         <v>1.6158841534971533</v>
       </c>
+      <c r="D60">
+        <v>15.41793226250881</v>
+      </c>
+      <c r="E60">
+        <v>1.2158589841201031</v>
+      </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A61" s="2" t="s">
         <v>27</v>
       </c>
@@ -8058,8 +8452,14 @@
       <c r="C61">
         <v>2.1362856073434378</v>
       </c>
+      <c r="D61">
+        <v>15.406716488533981</v>
+      </c>
+      <c r="E61">
+        <v>1.82113601164577</v>
+      </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A62" s="2" t="s">
         <v>28</v>
       </c>
@@ -8069,8 +8469,14 @@
       <c r="C62">
         <v>2.4567143353559051</v>
       </c>
+      <c r="D62">
+        <v>14.829682422442303</v>
+      </c>
+      <c r="E62">
+        <v>2.2497001572577777</v>
+      </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
         <v>29</v>
       </c>
@@ -8080,8 +8486,14 @@
       <c r="C63">
         <v>2.7533640552295995</v>
       </c>
+      <c r="D63">
+        <v>14.459804646745468</v>
+      </c>
+      <c r="E63">
+        <v>2.6735961153807559</v>
+      </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A64" s="2" t="s">
         <v>30</v>
       </c>
@@ -8091,8 +8503,14 @@
       <c r="C64">
         <v>2.8623666132066798</v>
       </c>
+      <c r="D64">
+        <v>13.725289492116069</v>
+      </c>
+      <c r="E64">
+        <v>2.8906480860794654</v>
+      </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65" s="2" t="s">
         <v>31</v>
       </c>
@@ -8102,8 +8520,14 @@
       <c r="C65">
         <v>2.949315215865068</v>
       </c>
+      <c r="D65">
+        <v>13.084701907070789</v>
+      </c>
+      <c r="E65">
+        <v>3.0649729931017586</v>
+      </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66" s="2" t="s">
         <v>32</v>
       </c>
@@ -8113,8 +8537,14 @@
       <c r="C66">
         <v>3.1977149593886267</v>
       </c>
+      <c r="D66">
+        <v>12.553135665548929</v>
+      </c>
+      <c r="E66">
+        <v>3.2240025580392877</v>
+      </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67" s="2" t="s">
         <v>33</v>
       </c>
@@ -8124,8 +8554,14 @@
       <c r="C67">
         <v>3.2384978512897011</v>
       </c>
+      <c r="D67">
+        <v>12.059121015447513</v>
+      </c>
+      <c r="E67">
+        <v>3.3471468154077755</v>
+      </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A68" s="2" t="s">
         <v>34</v>
       </c>
@@ -8134,6 +8570,12 @@
       </c>
       <c r="C68">
         <v>2.9528295234091897</v>
+      </c>
+      <c r="D68">
+        <v>11.510721826072064</v>
+      </c>
+      <c r="E68">
+        <v>3.3884888682617169</v>
       </c>
     </row>
   </sheetData>
@@ -8146,4 +8588,135 @@
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4389B7A4-719A-44B4-AFDF-2F90FB7E32A3}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2">
+        <v>126.8035321599082</v>
+      </c>
+      <c r="C2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>98.545912826763768</v>
+      </c>
+      <c r="C3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4">
+        <v>72.805856189522657</v>
+      </c>
+      <c r="C4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5">
+        <v>56.809365497268963</v>
+      </c>
+      <c r="C5">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6">
+        <v>45.095336024015737</v>
+      </c>
+      <c r="C6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7">
+        <v>38.913860226842672</v>
+      </c>
+      <c r="C7">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <v>34.328390656617458</v>
+      </c>
+      <c r="C8">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9">
+        <v>28.811277085008459</v>
+      </c>
+      <c r="C9">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10">
+        <v>25.81204633451021</v>
+      </c>
+      <c r="C10">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11">
+        <v>23.378376193182351</v>
+      </c>
+      <c r="C11">
+        <v>0.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>